<commit_message>
Added Jose's Mandatory Kindergarten data
</commit_message>
<xml_diff>
--- a/Analysis/Clean/00EducationAssignments.xlsx
+++ b/Analysis/Clean/00EducationAssignments.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="-135" windowWidth="28770" windowHeight="12945"/>
+    <workbookView xWindow="30" yWindow="-135" windowWidth="35085" windowHeight="12945"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="169">
   <si>
     <t>By State Information to use in the project</t>
   </si>
@@ -521,6 +521,12 @@
   </si>
   <si>
     <t>11restaurants_vf.csv</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/josequinonez/U11Homework/master/MandatoryKindergarten.csv?raw=true</t>
+  </si>
+  <si>
+    <t>05MandatoryKindergarten.csv</t>
   </si>
 </sst>
 </file>
@@ -694,7 +700,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -765,6 +771,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1076,7 +1083,7 @@
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection activeCell="A3" sqref="A3"/>
-      <selection pane="topRight" activeCell="G31" sqref="G31"/>
+      <selection pane="topRight" activeCell="R11" sqref="R11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -1449,8 +1456,12 @@
         <v>45</v>
       </c>
       <c r="D11" s="11"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="35"/>
+      <c r="E11" s="42" t="s">
+        <v>167</v>
+      </c>
+      <c r="F11" s="35" t="s">
+        <v>168</v>
+      </c>
       <c r="G11" s="9" t="str">
         <f t="shared" si="0"/>
         <v>ClickToOpen</v>
@@ -1465,11 +1476,11 @@
       <c r="O11" s="31"/>
       <c r="R11" s="18" t="str">
         <f t="shared" si="1"/>
-        <v>Proc Import Out = i(KEEP =   )datafile = "\\client\c$\Users\anobs\Documents\GitHub\Unit11SATACT\Analysis\Stage4Import\"</v>
+        <v>Proc Import Out = i05MandatoryKindergarten_csv(KEEP =   )datafile = "\\client\c$\Users\anobs\Documents\GitHub\Unit11SATACT\Analysis\Stage4Import\05MandatoryKindergarten.csv"</v>
       </c>
       <c r="S11" s="18" t="str">
         <f t="shared" si="2"/>
-        <v>datafile = "\\client\c$\Users\anobs\Documents\GitHub\Unit11SATACT\Analysis\Stage4Import\"</v>
+        <v>datafile = "\\client\c$\Users\anobs\Documents\GitHub\Unit11SATACT\Analysis\Stage4Import\05MandatoryKindergarten.csv"</v>
       </c>
       <c r="U11" s="18" t="str">
         <f t="shared" si="3"/>
@@ -2646,9 +2657,10 @@
     <hyperlink ref="E31" r:id="rId27"/>
     <hyperlink ref="E15" r:id="rId28"/>
     <hyperlink ref="D15" r:id="rId29"/>
+    <hyperlink ref="E11" r:id="rId30"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="65" orientation="portrait" r:id="rId30"/>
+  <pageSetup scale="65" orientation="portrait" r:id="rId31"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
fixed hyperlinks in Education Assignment.xlsx
</commit_message>
<xml_diff>
--- a/Analysis/Clean/00EducationAssignments.xlsx
+++ b/Analysis/Clean/00EducationAssignments.xlsx
@@ -762,6 +762,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -771,7 +772,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1083,7 +1083,7 @@
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection activeCell="A3" sqref="A3"/>
-      <selection pane="topRight" activeCell="R11" sqref="R11"/>
+      <selection pane="topRight" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -1110,11 +1110,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:24" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
       <c r="E2" s="1"/>
       <c r="G2" s="2" t="s">
         <v>144</v>
@@ -1131,15 +1131,15 @@
       <c r="E3" t="s">
         <v>150</v>
       </c>
-      <c r="G3" s="39" t="s">
+      <c r="G3" s="40" t="s">
         <v>159</v>
       </c>
-      <c r="H3" s="40"/>
-      <c r="I3" s="40"/>
-      <c r="J3" s="40"/>
-      <c r="K3" s="40"/>
-      <c r="L3" s="40"/>
-      <c r="M3" s="40"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="41"/>
+      <c r="K3" s="41"/>
+      <c r="L3" s="41"/>
+      <c r="M3" s="41"/>
       <c r="S3" t="str">
         <f>SUBSTITUTE($G$3,"C:\","\\client\c$\")&amp;"\"</f>
         <v>\\client\c$\Users\anobs\Documents\GitHub\Unit11SATACT\Analysis\Stage4Import\</v>
@@ -1152,7 +1152,7 @@
       <c r="B4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="37" t="s">
+      <c r="C4" s="38" t="s">
         <v>17</v>
       </c>
       <c r="D4" s="3"/>
@@ -1162,7 +1162,7 @@
       <c r="B5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="37"/>
+      <c r="C5" s="38"/>
       <c r="D5" s="15" t="s">
         <v>89</v>
       </c>
@@ -1190,7 +1190,7 @@
       <c r="B6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="38"/>
+      <c r="C6" s="39"/>
       <c r="D6" s="14"/>
       <c r="E6" s="13"/>
       <c r="F6" s="13"/>
@@ -1456,7 +1456,7 @@
         <v>45</v>
       </c>
       <c r="D11" s="11"/>
-      <c r="E11" s="42" t="s">
+      <c r="E11" s="37" t="s">
         <v>167</v>
       </c>
       <c r="F11" s="35" t="s">
@@ -2658,9 +2658,12 @@
     <hyperlink ref="E15" r:id="rId28"/>
     <hyperlink ref="D15" r:id="rId29"/>
     <hyperlink ref="E11" r:id="rId30"/>
+    <hyperlink ref="D29" r:id="rId31"/>
+    <hyperlink ref="D23" r:id="rId32"/>
+    <hyperlink ref="D21" r:id="rId33"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="65" orientation="portrait" r:id="rId31"/>
+  <pageSetup scale="65" orientation="portrait" r:id="rId34"/>
 </worksheet>
 </file>
 

</xml_diff>